<commit_message>
Updates solenoid channel assignments to match Robot Pinout.
</commit_message>
<xml_diff>
--- a/2019 Competition Robot Pinout.xlsx
+++ b/2019 Competition Robot Pinout.xlsx
@@ -1,22 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wentzdr\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blzzrd\git\2019-RobotCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{F2BA0627-CDCF-4D11-B190-6C39742556DE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13440" windowHeight="6285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13440" windowHeight="6288"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
   <si>
     <t>PDP Channel</t>
   </si>
@@ -194,12 +192,27 @@
   </si>
   <si>
     <t>Hatch Claw Release</t>
+  </si>
+  <si>
+    <t>Ball Intake Motor</t>
+  </si>
+  <si>
+    <t>Ball Arm Raise</t>
+  </si>
+  <si>
+    <t>Ball Arm Lower</t>
+  </si>
+  <si>
+    <t>Frame Stand Raise</t>
+  </si>
+  <si>
+    <t>Frame Stand Lower</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -272,9 +285,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -288,6 +298,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -569,559 +582,569 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="22.28515625" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="4.5703125" customWidth="1"/>
+    <col min="1" max="1" width="22.26171875" customWidth="1"/>
+    <col min="2" max="2" width="10.41796875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="4.578125" customWidth="1"/>
     <col min="5" max="5" width="29" customWidth="1"/>
-    <col min="8" max="8" width="1.28515625" customWidth="1"/>
+    <col min="8" max="8" width="1.26171875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:7" ht="23.1" x14ac:dyDescent="0.85">
+      <c r="A1" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-    </row>
-    <row r="2" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+    </row>
+    <row r="2" spans="1:7" ht="23.1" x14ac:dyDescent="0.85">
       <c r="A2" s="2"/>
     </row>
-    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+    <row r="3" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+      <c r="A3" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G3" s="9" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="4">
         <v>0</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="4">
         <v>0</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="4">
         <v>0</v>
       </c>
-      <c r="G4" s="5"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="G4" s="4"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="6">
         <v>1</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="6">
         <v>1</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="6">
         <f>F4+1</f>
         <v>1</v>
       </c>
-      <c r="G5" s="7"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="G5" s="6"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="4">
         <v>2</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="4">
         <v>2</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="4">
         <f t="shared" ref="F6:F29" si="0">F5+1</f>
         <v>2</v>
       </c>
-      <c r="G6" s="5"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+      <c r="G6" s="4"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7" s="6">
         <v>3</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="6">
         <v>3</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="6">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="G7" s="7"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="G7" s="6"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="4">
         <v>4</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="4">
         <v>4</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="4">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="G8" s="5"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+      <c r="G8" s="4"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B9" s="6">
         <v>5</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="6">
         <v>5</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="7">
+      <c r="F9" s="6">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G9" s="7"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+      <c r="G9" s="6"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10" s="4">
         <v>6</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="4">
         <v>6</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="4">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="G10" s="5"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+      <c r="G10" s="4"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="7">
+      <c r="B11" s="6">
         <v>7</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="6">
         <v>7</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E11" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F11" s="6">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="G11" s="7"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+      <c r="G11" s="6"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="5">
+      <c r="B12" s="4">
         <v>8</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="4">
         <v>8</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F12" s="4">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="G12" s="5"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
+      <c r="G12" s="4"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="7">
+      <c r="B13" s="6">
         <v>9</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C13" s="6">
         <v>9</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="E13" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="F13" s="7">
+      <c r="F13" s="6">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="G13" s="7"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+      <c r="G13" s="6"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B14" s="4">
         <v>10</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14" s="4">
         <v>10</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E14" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="F14" s="5">
+      <c r="F14" s="4">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G14" s="5">
+      <c r="G14" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="7">
+      <c r="B15" s="6">
         <v>11</v>
       </c>
-      <c r="C15" s="7">
+      <c r="C15" s="6">
         <v>11</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="E15" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F15" s="7">
+      <c r="F15" s="6">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="G15" s="7">
+      <c r="G15" s="6">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="5">
+      <c r="B16" s="4">
         <v>12</v>
       </c>
-      <c r="C16" s="5">
+      <c r="C16" s="4">
         <v>12</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E16" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="F16" s="5">
+      <c r="F16" s="4">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="G16" s="5">
+      <c r="G16" s="4">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="7">
+      <c r="B17" s="6">
         <v>13</v>
       </c>
-      <c r="C17" s="7">
+      <c r="C17" s="6">
         <v>13</v>
       </c>
-      <c r="E17" s="6" t="s">
+      <c r="E17" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="F17" s="7">
+      <c r="F17" s="6">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="G17" s="7">
+      <c r="G17" s="6">
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
-      <c r="B18" s="5">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B18" s="4">
         <v>14</v>
       </c>
-      <c r="C18" s="5">
+      <c r="C18" s="4">
         <v>14</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="E18" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F18" s="5">
+      <c r="F18" s="4">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="G18" s="5"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
-      <c r="B19" s="7">
+      <c r="G18" s="4"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="5"/>
+      <c r="B19" s="6">
         <v>15</v>
       </c>
-      <c r="C19" s="7">
+      <c r="C19" s="6">
         <v>15</v>
       </c>
-      <c r="E19" s="6" t="s">
+      <c r="E19" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="F19" s="7">
+      <c r="F19" s="6">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="G19" s="7"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E20" s="4" t="s">
+      <c r="G19" s="6"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="E20" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F20" s="5">
+      <c r="F20" s="4">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="G20" s="5"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E21" s="6" t="s">
+      <c r="G20" s="4"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="E21" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F21" s="7">
+      <c r="F21" s="6">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="G21" s="7"/>
-    </row>
-    <row r="22" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="10" t="s">
+      <c r="G21" s="6"/>
+    </row>
+    <row r="22" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+      <c r="A22" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="B22" s="10" t="s">
+      <c r="B22" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="E22" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F22" s="5">
+      <c r="F22" s="4">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="G22" s="5">
+      <c r="G22" s="4">
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B23" s="5">
+      <c r="B23" s="4">
         <v>0</v>
       </c>
-      <c r="E23" s="6" t="s">
+      <c r="E23" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="F23" s="7">
+      <c r="F23" s="6">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="G23" s="7">
+      <c r="G23" s="6">
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B24" s="7">
+      <c r="B24" s="6">
         <v>1</v>
       </c>
-      <c r="E24" s="8" t="s">
+      <c r="E24" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="F24" s="9">
+      <c r="F24" s="8">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="G24" s="9">
+      <c r="G24" s="8">
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B25" s="5">
+      <c r="B25" s="4">
         <v>2</v>
       </c>
-      <c r="E25" s="6" t="s">
+      <c r="E25" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="F25" s="7">
+      <c r="F25" s="6">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="G25" s="7">
+      <c r="G25" s="6">
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="6" t="s">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B26" s="7">
+      <c r="B26" s="6">
         <v>3</v>
       </c>
-      <c r="E26" s="4" t="s">
+      <c r="E26" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="F26" s="5">
+      <c r="F26" s="4">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="G26" s="5">
+      <c r="G26" s="4">
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E27" s="6"/>
-      <c r="F27" s="7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="E27" s="5"/>
+      <c r="F27" s="6">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="G27" s="7">
+      <c r="G27" s="6">
         <v>19</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E28" s="4"/>
-      <c r="F28" s="5">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="E28" s="3"/>
+      <c r="F28" s="4">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="G28" s="5"/>
-    </row>
-    <row r="29" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="10" t="s">
+      <c r="G28" s="4"/>
+    </row>
+    <row r="29" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+      <c r="A29" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="B29" s="10" t="s">
+      <c r="B29" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="E29" s="6"/>
-      <c r="F29" s="7">
+      <c r="E29" s="5"/>
+      <c r="F29" s="6">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="G29" s="7"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
+      <c r="G29" s="6"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B30" s="5">
+      <c r="B30" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="6" t="s">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B31" s="7">
+      <c r="B31" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="4" t="s">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B32" s="5">
+      <c r="B32" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="6" t="s">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B33" s="7">
+      <c r="B33" s="6">
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="4"/>
-      <c r="B34" s="5">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B34" s="4">
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="6"/>
-      <c r="B35" s="7">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B35" s="6">
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="4"/>
-      <c r="B36" s="5">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B36" s="4">
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="6"/>
-      <c r="B37" s="7">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B37" s="6">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adds ball intake motor encoder
</commit_message>
<xml_diff>
--- a/2019 Competition Robot Pinout.xlsx
+++ b/2019 Competition Robot Pinout.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
   <si>
     <t>PDP Channel</t>
   </si>
@@ -207,6 +207,12 @@
   </si>
   <si>
     <t>Frame Stand Lower</t>
+  </si>
+  <si>
+    <t>Ball Intake Motor Encoder A</t>
+  </si>
+  <si>
+    <t>Ball Intake Motor Encoder B</t>
   </si>
 </sst>
 </file>
@@ -585,8 +591,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1053,7 +1059,9 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="E27" s="5"/>
+      <c r="E27" s="5" t="s">
+        <v>61</v>
+      </c>
       <c r="F27" s="6">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -1063,7 +1071,9 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="E28" s="3"/>
+      <c r="E28" s="3" t="s">
+        <v>62</v>
+      </c>
       <c r="F28" s="4">
         <f t="shared" si="0"/>
         <v>24</v>

</xml_diff>